<commit_message>
UI changes, and further development
</commit_message>
<xml_diff>
--- a/Symbols.xlsx
+++ b/Symbols.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Williams\Programming\ENMT211-Elevator-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662140E2-5E0A-4B3B-81B8-006094BEF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70891D15-D86A-49C9-9397-B94BF6398E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13095" yWindow="0" windowWidth="25410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Description</t>
   </si>
@@ -75,9 +86,6 @@
     <t>Current Floor</t>
   </si>
   <si>
-    <t>State Stationary</t>
-  </si>
-  <si>
     <t>State Traversing</t>
   </si>
   <si>
@@ -246,13 +254,34 @@
     <t>Sample Period</t>
   </si>
   <si>
-    <t>Inverse Kp</t>
-  </si>
-  <si>
-    <t>Inverse Ki</t>
-  </si>
-  <si>
-    <t>Inverse Kd</t>
+    <t>Elevator Position</t>
+  </si>
+  <si>
+    <t>+ve Inverse Kp</t>
+  </si>
+  <si>
+    <t>+ve Inverse Ki</t>
+  </si>
+  <si>
+    <t>+ve Inverse Kd</t>
+  </si>
+  <si>
+    <t>-ve Inverse Kp</t>
+  </si>
+  <si>
+    <t>-ve Inverse Ki</t>
+  </si>
+  <si>
+    <t>-ve Inverse Kd</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>State Loading</t>
+  </si>
+  <si>
+    <t>State Idle</t>
   </si>
 </sst>
 </file>
@@ -373,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,16 +414,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -677,18 +710,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" style="1" customWidth="1"/>
-    <col min="3" max="19" width="18.28515625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="22" width="18.28515625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -752,883 +785,912 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
+      <c r="D4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="E5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="8"/>
+      <c r="G17" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N17" s="8"/>
+      <c r="O17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P17" s="8"/>
+      <c r="Q17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R17" s="8"/>
+      <c r="S17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="T17" s="8"/>
+      <c r="U17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="V17" s="8"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>1</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>2</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="6">
         <v>5</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="6">
         <v>4</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="6">
         <v>3</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="6">
         <v>2</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="6">
         <v>1</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="3" t="s">
+      <c r="H21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>100</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>101</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>102</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>103</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="6">
         <v>5</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="6">
         <v>4</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="6">
         <v>3</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="6">
         <v>2</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="6">
         <v>1</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" s="3" t="s">
+      <c r="H26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>210</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="8"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2012,7 +2074,8 @@
       <c r="A51" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="U17:V17"/>
     <mergeCell ref="C27:S27"/>
     <mergeCell ref="C28:S28"/>
     <mergeCell ref="C17:D17"/>
@@ -2020,6 +2083,9 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>